<commit_message>
Matrice FINAL VRAIMENT VRAI
</commit_message>
<xml_diff>
--- a/Matrice projetfinis.xlsx
+++ b/Matrice projetfinis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>ID_potion</t>
   </si>
@@ -101,9 +101,6 @@
     <t>v</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>Quantite_potion</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>prix_onguent</t>
+  </si>
+  <si>
+    <t>Quantité_stock</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:AY51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AX50" sqref="A1:AX50"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +912,7 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1373,7 +1373,9 @@
       <c r="AX11" s="5"/>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1387,9 +1389,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="12"/>
-      <c r="M12" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="M12" s="3"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1444,9 +1444,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="12"/>
-      <c r="N13" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="N13" s="3"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1503,9 +1501,7 @@
       <c r="N14" s="12">
         <v>1</v>
       </c>
-      <c r="O14" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="O14" s="13"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1544,7 +1540,7 @@
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1600,7 +1596,7 @@
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1656,7 +1652,7 @@
     </row>
     <row r="17" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1676,9 +1672,7 @@
       <c r="Q17" s="12">
         <v>1</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="R17" s="3"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
@@ -1735,9 +1729,7 @@
         <v>1</v>
       </c>
       <c r="R18" s="12"/>
-      <c r="S18" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="S18" s="3"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
@@ -1794,9 +1786,7 @@
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="12"/>
-      <c r="T19" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="T19" s="3"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
@@ -1853,9 +1843,7 @@
       <c r="T20" s="12">
         <v>1</v>
       </c>
-      <c r="U20" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="U20" s="3"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
@@ -1914,9 +1902,7 @@
       <c r="U21" s="12">
         <v>1</v>
       </c>
-      <c r="V21" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="V21" s="3"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
@@ -1975,9 +1961,7 @@
         <v>1</v>
       </c>
       <c r="V22" s="12"/>
-      <c r="W22" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="W22" s="3"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
@@ -2008,7 +1992,7 @@
     </row>
     <row r="23" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2036,9 +2020,7 @@
       </c>
       <c r="V23" s="2"/>
       <c r="W23" s="12"/>
-      <c r="X23" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="X23" s="3"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
@@ -2068,7 +2050,7 @@
     </row>
     <row r="24" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2095,9 +2077,7 @@
       <c r="X24" s="12">
         <v>1</v>
       </c>
-      <c r="Y24" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="Y24" s="3"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
@@ -2154,9 +2134,7 @@
         <v>1</v>
       </c>
       <c r="Y25" s="12"/>
-      <c r="Z25" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="Z25" s="3"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
@@ -2213,9 +2191,7 @@
       </c>
       <c r="Y26" s="2"/>
       <c r="Z26" s="12"/>
-      <c r="AA26" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="AA26" s="3"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
@@ -2242,7 +2218,7 @@
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2272,9 +2248,7 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
       <c r="AA27" s="12"/>
-      <c r="AB27" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="AB27" s="3"/>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
@@ -2300,7 +2274,7 @@
     </row>
     <row r="28" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2698,7 +2672,7 @@
     </row>
     <row r="35" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2757,7 +2731,7 @@
     </row>
     <row r="36" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3103,7 +3077,7 @@
     </row>
     <row r="42" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3162,7 +3136,7 @@
     </row>
     <row r="43" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3219,7 +3193,7 @@
     </row>
     <row r="44" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3276,7 +3250,7 @@
     </row>
     <row r="45" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3333,7 +3307,7 @@
     </row>
     <row r="46" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3390,7 +3364,7 @@
     </row>
     <row r="47" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3447,7 +3421,7 @@
     </row>
     <row r="48" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3504,7 +3478,7 @@
     </row>
     <row r="49" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3559,7 +3533,7 @@
     </row>
     <row r="50" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>

</xml_diff>

<commit_message>
MATRICE VRMT VRMT VRMT FINIS
</commit_message>
<xml_diff>
--- a/Matrice projetfinis.xlsx
+++ b/Matrice projetfinis.xlsx
@@ -173,7 +173,7 @@
     <t>prix_onguent</t>
   </si>
   <si>
-    <t>Quantité_stock</t>
+    <t>Quantite_stock</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:AY51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
MATRICE FINAL QUASIMENT SUR
</commit_message>
<xml_diff>
--- a/Matrice projetfinis.xlsx
+++ b/Matrice projetfinis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>ID_potion</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Quantite_stock</t>
+  </si>
+  <si>
+    <t>Recette</t>
   </si>
 </sst>
 </file>
@@ -627,26 +630,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY51"/>
+  <dimension ref="A1:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.44140625" customWidth="1"/>
-    <col min="13" max="36" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.44140625" customWidth="1"/>
-    <col min="38" max="49" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="3.44140625" customWidth="1"/>
-    <col min="51" max="51" width="3.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="2.33203125" customWidth="1"/>
+    <col min="7" max="9" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.44140625" customWidth="1"/>
+    <col min="14" max="37" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.44140625" customWidth="1"/>
+    <col min="39" max="50" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3.44140625" customWidth="1"/>
+    <col min="52" max="52" width="3.44140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4">
         <v>2</v>
@@ -795,8 +798,11 @@
       <c r="AX1" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AY1" s="4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -850,9 +856,10 @@
       <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2"/>
-      <c r="AX2" s="5"/>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="5"/>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -908,9 +915,10 @@
       <c r="AU3" s="2"/>
       <c r="AV3" s="2"/>
       <c r="AW3" s="2"/>
-      <c r="AX3" s="5"/>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="5"/>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
@@ -966,9 +974,10 @@
       <c r="AU4" s="2"/>
       <c r="AV4" s="2"/>
       <c r="AW4" s="2"/>
-      <c r="AX4" s="5"/>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="5"/>
+    </row>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -982,7 +991,7 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1026,19 +1035,20 @@
       <c r="AU5" s="2"/>
       <c r="AV5" s="2"/>
       <c r="AW5" s="2"/>
-      <c r="AX5" s="5"/>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="5"/>
+    </row>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1082,21 +1092,20 @@
       <c r="AU6" s="2"/>
       <c r="AV6" s="2"/>
       <c r="AW6" s="2"/>
-      <c r="AX6" s="5"/>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="5"/>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1">
+        <v>1</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1140,18 +1149,21 @@
       <c r="AU7" s="2"/>
       <c r="AV7" s="2"/>
       <c r="AW7" s="2"/>
-      <c r="AX7" s="5"/>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="5"/>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
       <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1196,11 +1208,12 @@
       <c r="AU8" s="2"/>
       <c r="AV8" s="2"/>
       <c r="AW8" s="2"/>
-      <c r="AX8" s="5"/>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="5"/>
+    </row>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1208,9 +1221,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1254,11 +1265,12 @@
       <c r="AU9" s="2"/>
       <c r="AV9" s="2"/>
       <c r="AW9" s="2"/>
-      <c r="AX9" s="5"/>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="5"/>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1266,10 +1278,10 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
       <c r="J10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1312,11 +1324,12 @@
       <c r="AU10" s="2"/>
       <c r="AV10" s="2"/>
       <c r="AW10" s="2"/>
-      <c r="AX10" s="5"/>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="5"/>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1324,15 +1337,15 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
       <c r="J11" s="2"/>
       <c r="K11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="13"/>
+      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1370,11 +1383,12 @@
       <c r="AU11" s="2"/>
       <c r="AV11" s="2"/>
       <c r="AW11" s="2"/>
-      <c r="AX11" s="5"/>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="5"/>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1382,14 +1396,16 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="3">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="3"/>
+      <c r="L12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="13"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
@@ -1426,11 +1442,12 @@
       <c r="AU12" s="2"/>
       <c r="AV12" s="2"/>
       <c r="AW12" s="2"/>
-      <c r="AX12" s="5"/>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="5"/>
+    </row>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1439,7 +1456,9 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1480,11 +1499,12 @@
       <c r="AU13" s="2"/>
       <c r="AV13" s="2"/>
       <c r="AW13" s="2"/>
-      <c r="AX13" s="5"/>
-    </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="5"/>
+    </row>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1498,10 +1518,8 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="12">
-        <v>1</v>
-      </c>
-      <c r="O14" s="13"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="3"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1536,11 +1554,12 @@
       <c r="AU14" s="2"/>
       <c r="AV14" s="2"/>
       <c r="AW14" s="2"/>
-      <c r="AX14" s="5"/>
-    </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="5"/>
+    </row>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1554,10 +1573,10 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2">
-        <v>1</v>
-      </c>
-      <c r="O15" s="12"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="12">
+        <v>1</v>
+      </c>
       <c r="P15" s="13"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1592,11 +1611,12 @@
       <c r="AU15" s="2"/>
       <c r="AV15" s="2"/>
       <c r="AW15" s="2"/>
-      <c r="AX15" s="5"/>
-    </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="5"/>
+    </row>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1610,10 +1630,10 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="2">
-        <v>1</v>
-      </c>
-      <c r="O16" s="3"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2">
+        <v>1</v>
+      </c>
       <c r="P16" s="12"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="2"/>
@@ -1648,11 +1668,12 @@
       <c r="AU16" s="2"/>
       <c r="AV16" s="2"/>
       <c r="AW16" s="2"/>
-      <c r="AX16" s="5"/>
-    </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="5"/>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1667,12 +1688,12 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="3"/>
+      <c r="O17" s="2">
+        <v>1</v>
+      </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="12">
-        <v>1</v>
-      </c>
-      <c r="R17" s="3"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="13"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
@@ -1704,11 +1725,12 @@
       <c r="AU17" s="2"/>
       <c r="AV17" s="2"/>
       <c r="AW17" s="2"/>
-      <c r="AX17" s="5"/>
-    </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX17" s="2"/>
+      <c r="AY17" s="5"/>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1724,11 +1746,11 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2">
-        <v>1</v>
-      </c>
-      <c r="R18" s="12"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="12">
+        <v>1</v>
+      </c>
       <c r="S18" s="3"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
@@ -1760,11 +1782,12 @@
       <c r="AU18" s="2"/>
       <c r="AV18" s="2"/>
       <c r="AW18" s="2"/>
-      <c r="AX18" s="5"/>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="5"/>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1781,10 +1804,10 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
-      <c r="Q19" s="2">
-        <v>1</v>
-      </c>
-      <c r="R19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
       <c r="S19" s="12"/>
       <c r="T19" s="3"/>
       <c r="U19" s="2"/>
@@ -1816,11 +1839,12 @@
       <c r="AU19" s="2"/>
       <c r="AV19" s="2"/>
       <c r="AW19" s="2"/>
-      <c r="AX19" s="5"/>
-    </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX19" s="2"/>
+      <c r="AY19" s="5"/>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1838,11 +1862,11 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
       <c r="S20" s="2"/>
-      <c r="T20" s="12">
-        <v>1</v>
-      </c>
+      <c r="T20" s="12"/>
       <c r="U20" s="3"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
@@ -1872,11 +1896,12 @@
       <c r="AU20" s="2"/>
       <c r="AV20" s="2"/>
       <c r="AW20" s="2"/>
-      <c r="AX20" s="5"/>
-    </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX20" s="2"/>
+      <c r="AY20" s="5"/>
+    </row>
+    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1896,9 +1921,7 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
-      <c r="T21" s="2">
-        <v>1</v>
-      </c>
+      <c r="T21" s="2"/>
       <c r="U21" s="12">
         <v>1</v>
       </c>
@@ -1930,11 +1953,12 @@
       <c r="AU21" s="2"/>
       <c r="AV21" s="2"/>
       <c r="AW21" s="2"/>
-      <c r="AX21" s="5"/>
-    </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="5"/>
+    </row>
+    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1954,13 +1978,13 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
-      <c r="T22" s="2">
-        <v>1</v>
-      </c>
+      <c r="T22" s="2"/>
       <c r="U22" s="2">
         <v>1</v>
       </c>
-      <c r="V22" s="12"/>
+      <c r="V22" s="12">
+        <v>1</v>
+      </c>
       <c r="W22" s="3"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
@@ -1988,11 +2012,12 @@
       <c r="AU22" s="2"/>
       <c r="AV22" s="2"/>
       <c r="AW22" s="2"/>
-      <c r="AX22" s="5"/>
-    </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX22" s="2"/>
+      <c r="AY22" s="5"/>
+    </row>
+    <row r="23" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2012,13 +2037,13 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
-      <c r="T23" s="3">
-        <v>1</v>
-      </c>
+      <c r="T23" s="2"/>
       <c r="U23" s="2">
         <v>1</v>
       </c>
-      <c r="V23" s="2"/>
+      <c r="V23" s="2">
+        <v>1</v>
+      </c>
       <c r="W23" s="12"/>
       <c r="X23" s="3"/>
       <c r="Y23" s="2"/>
@@ -2046,11 +2071,12 @@
       <c r="AU23" s="2"/>
       <c r="AV23" s="2"/>
       <c r="AW23" s="2"/>
-      <c r="AX23" s="5"/>
-    </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX23" s="2"/>
+      <c r="AY23" s="5"/>
+    </row>
+    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2071,12 +2097,14 @@
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
+      <c r="U24" s="3">
+        <v>1</v>
+      </c>
+      <c r="V24" s="2">
+        <v>1</v>
+      </c>
       <c r="W24" s="2"/>
-      <c r="X24" s="12">
-        <v>1</v>
-      </c>
+      <c r="X24" s="12"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
@@ -2102,11 +2130,12 @@
       <c r="AU24" s="2"/>
       <c r="AV24" s="2"/>
       <c r="AW24" s="2"/>
-      <c r="AX24" s="5"/>
-    </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX24" s="2"/>
+      <c r="AY24" s="5"/>
+    </row>
+    <row r="25" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2130,10 +2159,10 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
-      <c r="X25" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="12"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="12">
+        <v>1</v>
+      </c>
       <c r="Z25" s="3"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
@@ -2158,11 +2187,12 @@
       <c r="AU25" s="2"/>
       <c r="AV25" s="2"/>
       <c r="AW25" s="2"/>
-      <c r="AX25" s="5"/>
-    </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="5"/>
+    </row>
+    <row r="26" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2186,10 +2216,10 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
-      <c r="X26" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2">
+        <v>1</v>
+      </c>
       <c r="Z26" s="12"/>
       <c r="AA26" s="3"/>
       <c r="AB26" s="2"/>
@@ -2214,11 +2244,12 @@
       <c r="AU26" s="2"/>
       <c r="AV26" s="2"/>
       <c r="AW26" s="2"/>
-      <c r="AX26" s="5"/>
-    </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="5"/>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2242,10 +2273,10 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
-      <c r="X27" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2">
+        <v>1</v>
+      </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="12"/>
       <c r="AB27" s="3"/>
@@ -2270,11 +2301,12 @@
       <c r="AU27" s="2"/>
       <c r="AV27" s="2"/>
       <c r="AW27" s="2"/>
-      <c r="AX27" s="5"/>
-    </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX27" s="2"/>
+      <c r="AY27" s="5"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2298,17 +2330,17 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
-      <c r="X28" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="3">
+        <v>1</v>
+      </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="12"/>
       <c r="AC28" s="3"/>
-      <c r="AD28" s="3"/>
-      <c r="AE28" s="3"/>
-      <c r="AF28" s="3"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
@@ -2326,11 +2358,12 @@
       <c r="AU28" s="2"/>
       <c r="AV28" s="2"/>
       <c r="AW28" s="2"/>
-      <c r="AX28" s="5"/>
-    </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX28" s="2"/>
+      <c r="AY28" s="5"/>
+    </row>
+    <row r="29" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2355,39 +2388,39 @@
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
-      <c r="Y29" s="2"/>
+      <c r="Y29" s="3">
+        <v>1</v>
+      </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
-      <c r="AB29" s="3"/>
-      <c r="AC29" s="12">
-        <v>1</v>
-      </c>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="12"/>
       <c r="AD29" s="3"/>
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
-      <c r="AG29" s="2"/>
-      <c r="AH29" s="3"/>
-      <c r="AI29" s="3"/>
-      <c r="AJ29" s="3"/>
-      <c r="AK29" s="3"/>
-      <c r="AL29" s="3"/>
-      <c r="AM29" s="3"/>
-      <c r="AN29" s="3"/>
-      <c r="AO29" s="3"/>
-      <c r="AP29" s="3"/>
-      <c r="AQ29" s="3"/>
-      <c r="AR29" s="3"/>
-      <c r="AS29" s="3"/>
-      <c r="AT29" s="3"/>
-      <c r="AU29" s="3"/>
-      <c r="AV29" s="3"/>
-      <c r="AW29" s="3"/>
-      <c r="AX29" s="6"/>
-      <c r="AY29" s="3"/>
-    </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+      <c r="AJ29" s="2"/>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="2"/>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
+      <c r="AP29" s="2"/>
+      <c r="AQ29" s="2"/>
+      <c r="AR29" s="2"/>
+      <c r="AS29" s="2"/>
+      <c r="AT29" s="2"/>
+      <c r="AU29" s="2"/>
+      <c r="AV29" s="2"/>
+      <c r="AW29" s="2"/>
+      <c r="AX29" s="2"/>
+      <c r="AY29" s="5"/>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2415,15 +2448,15 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
-      <c r="AB30" s="3"/>
-      <c r="AC30" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD30" s="12"/>
-      <c r="AE30" s="13"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
-      <c r="AG30" s="2"/>
-      <c r="AH30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="2"/>
       <c r="AI30" s="3"/>
       <c r="AJ30" s="3"/>
       <c r="AK30" s="3"/>
@@ -2439,12 +2472,13 @@
       <c r="AU30" s="3"/>
       <c r="AV30" s="3"/>
       <c r="AW30" s="3"/>
-      <c r="AX30" s="6"/>
-      <c r="AY30" s="3"/>
-    </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX30" s="3"/>
+      <c r="AY30" s="6"/>
+      <c r="AZ30" s="3"/>
+    </row>
+    <row r="31" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2472,15 +2506,15 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
-      <c r="AB31" s="3"/>
-      <c r="AC31" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD31" s="3"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3">
+        <v>1</v>
+      </c>
       <c r="AE31" s="12"/>
-      <c r="AF31" s="3"/>
-      <c r="AG31" s="2"/>
-      <c r="AH31" s="3"/>
+      <c r="AF31" s="13"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="2"/>
       <c r="AI31" s="3"/>
       <c r="AJ31" s="3"/>
       <c r="AK31" s="3"/>
@@ -2496,12 +2530,13 @@
       <c r="AU31" s="3"/>
       <c r="AV31" s="3"/>
       <c r="AW31" s="3"/>
-      <c r="AX31" s="6"/>
-      <c r="AY31" s="3"/>
-    </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX31" s="3"/>
+      <c r="AY31" s="6"/>
+      <c r="AZ31" s="3"/>
+    </row>
+    <row r="32" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2529,15 +2564,15 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
-      <c r="AB32" s="3"/>
-      <c r="AC32" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD32" s="3"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3">
+        <v>1</v>
+      </c>
       <c r="AE32" s="3"/>
-      <c r="AF32" s="1"/>
+      <c r="AF32" s="12"/>
       <c r="AG32" s="3"/>
-      <c r="AH32" s="3"/>
+      <c r="AH32" s="2"/>
       <c r="AI32" s="3"/>
       <c r="AJ32" s="3"/>
       <c r="AK32" s="3"/>
@@ -2553,12 +2588,13 @@
       <c r="AU32" s="3"/>
       <c r="AV32" s="3"/>
       <c r="AW32" s="3"/>
-      <c r="AX32" s="6"/>
-      <c r="AY32" s="3"/>
-    </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX32" s="3"/>
+      <c r="AY32" s="6"/>
+      <c r="AZ32" s="3"/>
+    </row>
+    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2586,14 +2622,14 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
-      <c r="AB33" s="3"/>
+      <c r="AB33" s="2"/>
       <c r="AC33" s="3"/>
-      <c r="AD33" s="3"/>
+      <c r="AD33" s="3">
+        <v>1</v>
+      </c>
       <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
-      <c r="AG33" s="1">
-        <v>1</v>
-      </c>
+      <c r="AG33" s="1"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
       <c r="AJ33" s="3"/>
@@ -2610,12 +2646,13 @@
       <c r="AU33" s="3"/>
       <c r="AV33" s="3"/>
       <c r="AW33" s="3"/>
-      <c r="AX33" s="6"/>
-      <c r="AY33" s="3"/>
-    </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX33" s="3"/>
+      <c r="AY33" s="6"/>
+      <c r="AZ33" s="3"/>
+    </row>
+    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2643,15 +2680,15 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
-      <c r="AB34" s="3"/>
+      <c r="AB34" s="2"/>
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
-      <c r="AG34" s="3">
-        <v>1</v>
-      </c>
-      <c r="AH34" s="1"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="1">
+        <v>1</v>
+      </c>
       <c r="AI34" s="3"/>
       <c r="AJ34" s="3"/>
       <c r="AK34" s="3"/>
@@ -2667,12 +2704,13 @@
       <c r="AU34" s="3"/>
       <c r="AV34" s="3"/>
       <c r="AW34" s="3"/>
-      <c r="AX34" s="6"/>
-      <c r="AY34" s="3"/>
-    </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX34" s="3"/>
+      <c r="AY34" s="6"/>
+      <c r="AZ34" s="3"/>
+    </row>
+    <row r="35" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2701,17 +2739,15 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
-      <c r="AC35" s="2"/>
-      <c r="AD35" s="2"/>
-      <c r="AE35" s="2"/>
-      <c r="AF35" s="2"/>
-      <c r="AG35" s="3">
-        <v>1</v>
-      </c>
-      <c r="AH35" s="3"/>
-      <c r="AI35" s="1">
-        <v>1</v>
-      </c>
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="3"/>
+      <c r="AG35" s="3"/>
+      <c r="AH35" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="1"/>
       <c r="AJ35" s="3"/>
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
@@ -2726,12 +2762,13 @@
       <c r="AU35" s="3"/>
       <c r="AV35" s="3"/>
       <c r="AW35" s="3"/>
-      <c r="AX35" s="6"/>
-      <c r="AY35" s="3"/>
-    </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX35" s="3"/>
+      <c r="AY35" s="6"/>
+      <c r="AZ35" s="3"/>
+    </row>
+    <row r="36" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2764,14 +2801,14 @@
       <c r="AD36" s="2"/>
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
-      <c r="AG36" s="3">
-        <v>1</v>
-      </c>
-      <c r="AH36" s="3"/>
-      <c r="AI36" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ36" s="1"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="1">
+        <v>1</v>
+      </c>
       <c r="AK36" s="3"/>
       <c r="AL36" s="3"/>
       <c r="AM36" s="3"/>
@@ -2785,12 +2822,13 @@
       <c r="AU36" s="3"/>
       <c r="AV36" s="3"/>
       <c r="AW36" s="3"/>
-      <c r="AX36" s="6"/>
-      <c r="AY36" s="3"/>
-    </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX36" s="3"/>
+      <c r="AY36" s="6"/>
+      <c r="AZ36" s="3"/>
+    </row>
+    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2824,12 +2862,14 @@
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
-      <c r="AH37" s="3"/>
+      <c r="AH37" s="3">
+        <v>1</v>
+      </c>
       <c r="AI37" s="3"/>
-      <c r="AJ37" s="3"/>
-      <c r="AK37" s="1">
-        <v>1</v>
-      </c>
+      <c r="AJ37" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK37" s="1"/>
       <c r="AL37" s="3"/>
       <c r="AM37" s="3"/>
       <c r="AN37" s="3"/>
@@ -2842,12 +2882,13 @@
       <c r="AU37" s="3"/>
       <c r="AV37" s="3"/>
       <c r="AW37" s="3"/>
-      <c r="AX37" s="6"/>
-      <c r="AY37" s="3"/>
-    </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX37" s="3"/>
+      <c r="AY37" s="6"/>
+      <c r="AZ37" s="3"/>
+    </row>
+    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2881,13 +2922,13 @@
       <c r="AE38" s="2"/>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
-      <c r="AH38" s="3"/>
+      <c r="AH38" s="2"/>
       <c r="AI38" s="3"/>
       <c r="AJ38" s="3"/>
-      <c r="AK38" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL38" s="1"/>
+      <c r="AK38" s="3"/>
+      <c r="AL38" s="1">
+        <v>1</v>
+      </c>
       <c r="AM38" s="3"/>
       <c r="AN38" s="3"/>
       <c r="AO38" s="3"/>
@@ -2899,12 +2940,13 @@
       <c r="AU38" s="3"/>
       <c r="AV38" s="3"/>
       <c r="AW38" s="3"/>
-      <c r="AX38" s="6"/>
-      <c r="AY38" s="3"/>
-    </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX38" s="3"/>
+      <c r="AY38" s="6"/>
+      <c r="AZ38" s="3"/>
+    </row>
+    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2938,13 +2980,13 @@
       <c r="AE39" s="2"/>
       <c r="AF39" s="2"/>
       <c r="AG39" s="2"/>
-      <c r="AH39" s="3"/>
+      <c r="AH39" s="2"/>
       <c r="AI39" s="3"/>
       <c r="AJ39" s="3"/>
-      <c r="AK39" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL39" s="3"/>
+      <c r="AK39" s="3"/>
+      <c r="AL39" s="3">
+        <v>1</v>
+      </c>
       <c r="AM39" s="1"/>
       <c r="AN39" s="3"/>
       <c r="AO39" s="3"/>
@@ -2956,12 +2998,13 @@
       <c r="AU39" s="3"/>
       <c r="AV39" s="3"/>
       <c r="AW39" s="3"/>
-      <c r="AX39" s="6"/>
-      <c r="AY39" s="3"/>
-    </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>21</v>
+      <c r="AX39" s="3"/>
+      <c r="AY39" s="6"/>
+      <c r="AZ39" s="3"/>
+    </row>
+    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2995,15 +3038,15 @@
       <c r="AE40" s="2"/>
       <c r="AF40" s="2"/>
       <c r="AG40" s="2"/>
-      <c r="AH40" s="3"/>
+      <c r="AH40" s="2"/>
       <c r="AI40" s="3"/>
       <c r="AJ40" s="3"/>
       <c r="AK40" s="3"/>
-      <c r="AL40" s="3"/>
+      <c r="AL40" s="3">
+        <v>1</v>
+      </c>
       <c r="AM40" s="3"/>
-      <c r="AN40" s="1">
-        <v>1</v>
-      </c>
+      <c r="AN40" s="1"/>
       <c r="AO40" s="3"/>
       <c r="AP40" s="3"/>
       <c r="AQ40" s="3"/>
@@ -3013,12 +3056,13 @@
       <c r="AU40" s="3"/>
       <c r="AV40" s="3"/>
       <c r="AW40" s="3"/>
-      <c r="AX40" s="6"/>
-      <c r="AY40" s="3"/>
-    </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX40" s="3"/>
+      <c r="AY40" s="6"/>
+      <c r="AZ40" s="3"/>
+    </row>
+    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3052,15 +3096,13 @@
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
-      <c r="AH41" s="3"/>
+      <c r="AH41" s="2"/>
       <c r="AI41" s="3"/>
       <c r="AJ41" s="3"/>
       <c r="AK41" s="3"/>
       <c r="AL41" s="3"/>
       <c r="AM41" s="3"/>
-      <c r="AN41" s="3">
-        <v>1</v>
-      </c>
+      <c r="AN41" s="3"/>
       <c r="AO41" s="1">
         <v>1</v>
       </c>
@@ -3072,12 +3114,13 @@
       <c r="AU41" s="3"/>
       <c r="AV41" s="3"/>
       <c r="AW41" s="3"/>
-      <c r="AX41" s="6"/>
-      <c r="AY41" s="3"/>
-    </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX41" s="3"/>
+      <c r="AY41" s="6"/>
+      <c r="AZ41" s="3"/>
+    </row>
+    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3111,19 +3154,19 @@
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
-      <c r="AH42" s="3"/>
+      <c r="AH42" s="2"/>
       <c r="AI42" s="3"/>
       <c r="AJ42" s="3"/>
       <c r="AK42" s="3"/>
       <c r="AL42" s="3"/>
       <c r="AM42" s="3"/>
-      <c r="AN42" s="3">
-        <v>1</v>
-      </c>
+      <c r="AN42" s="3"/>
       <c r="AO42" s="3">
         <v>1</v>
       </c>
-      <c r="AP42" s="1"/>
+      <c r="AP42" s="1">
+        <v>1</v>
+      </c>
       <c r="AQ42" s="3"/>
       <c r="AR42" s="3"/>
       <c r="AS42" s="3"/>
@@ -3131,12 +3174,13 @@
       <c r="AU42" s="3"/>
       <c r="AV42" s="3"/>
       <c r="AW42" s="3"/>
-      <c r="AX42" s="6"/>
-      <c r="AY42" s="3"/>
-    </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX42" s="3"/>
+      <c r="AY42" s="6"/>
+      <c r="AZ42" s="3"/>
+    </row>
+    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3170,30 +3214,33 @@
       <c r="AE43" s="2"/>
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
-      <c r="AH43" s="3"/>
+      <c r="AH43" s="2"/>
       <c r="AI43" s="3"/>
       <c r="AJ43" s="3"/>
       <c r="AK43" s="3"/>
       <c r="AL43" s="3"/>
       <c r="AM43" s="3"/>
       <c r="AN43" s="3"/>
-      <c r="AO43" s="3"/>
-      <c r="AP43" s="3"/>
-      <c r="AQ43" s="1">
-        <v>1</v>
-      </c>
+      <c r="AO43" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP43" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ43" s="1"/>
       <c r="AR43" s="3"/>
       <c r="AS43" s="3"/>
       <c r="AT43" s="3"/>
       <c r="AU43" s="3"/>
       <c r="AV43" s="3"/>
       <c r="AW43" s="3"/>
-      <c r="AX43" s="6"/>
-      <c r="AY43" s="3"/>
-    </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX43" s="3"/>
+      <c r="AY43" s="6"/>
+      <c r="AZ43" s="3"/>
+    </row>
+    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3227,7 +3274,7 @@
       <c r="AE44" s="2"/>
       <c r="AF44" s="2"/>
       <c r="AG44" s="2"/>
-      <c r="AH44" s="3"/>
+      <c r="AH44" s="2"/>
       <c r="AI44" s="3"/>
       <c r="AJ44" s="3"/>
       <c r="AK44" s="3"/>
@@ -3236,21 +3283,22 @@
       <c r="AN44" s="3"/>
       <c r="AO44" s="3"/>
       <c r="AP44" s="3"/>
-      <c r="AQ44" s="3">
-        <v>1</v>
-      </c>
-      <c r="AR44" s="1"/>
+      <c r="AQ44" s="3"/>
+      <c r="AR44" s="1">
+        <v>1</v>
+      </c>
       <c r="AS44" s="3"/>
       <c r="AT44" s="3"/>
       <c r="AU44" s="3"/>
       <c r="AV44" s="3"/>
       <c r="AW44" s="3"/>
-      <c r="AX44" s="6"/>
-      <c r="AY44" s="3"/>
-    </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX44" s="3"/>
+      <c r="AY44" s="6"/>
+      <c r="AZ44" s="3"/>
+    </row>
+    <row r="45" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3284,7 +3332,7 @@
       <c r="AE45" s="2"/>
       <c r="AF45" s="2"/>
       <c r="AG45" s="2"/>
-      <c r="AH45" s="3"/>
+      <c r="AH45" s="2"/>
       <c r="AI45" s="3"/>
       <c r="AJ45" s="3"/>
       <c r="AK45" s="3"/>
@@ -3293,21 +3341,22 @@
       <c r="AN45" s="3"/>
       <c r="AO45" s="3"/>
       <c r="AP45" s="3"/>
-      <c r="AQ45" s="3">
-        <v>1</v>
-      </c>
-      <c r="AR45" s="3"/>
+      <c r="AQ45" s="3"/>
+      <c r="AR45" s="3">
+        <v>1</v>
+      </c>
       <c r="AS45" s="1"/>
       <c r="AT45" s="3"/>
       <c r="AU45" s="3"/>
       <c r="AV45" s="3"/>
       <c r="AW45" s="3"/>
-      <c r="AX45" s="6"/>
-      <c r="AY45" s="3"/>
-    </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX45" s="3"/>
+      <c r="AY45" s="6"/>
+      <c r="AZ45" s="3"/>
+    </row>
+    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3341,7 +3390,7 @@
       <c r="AE46" s="2"/>
       <c r="AF46" s="2"/>
       <c r="AG46" s="2"/>
-      <c r="AH46" s="3"/>
+      <c r="AH46" s="2"/>
       <c r="AI46" s="3"/>
       <c r="AJ46" s="3"/>
       <c r="AK46" s="3"/>
@@ -3350,21 +3399,22 @@
       <c r="AN46" s="3"/>
       <c r="AO46" s="3"/>
       <c r="AP46" s="3"/>
-      <c r="AQ46" s="3">
-        <v>1</v>
-      </c>
-      <c r="AR46" s="3"/>
+      <c r="AQ46" s="3"/>
+      <c r="AR46" s="3">
+        <v>1</v>
+      </c>
       <c r="AS46" s="3"/>
       <c r="AT46" s="1"/>
       <c r="AU46" s="3"/>
       <c r="AV46" s="3"/>
       <c r="AW46" s="3"/>
-      <c r="AX46" s="6"/>
-      <c r="AY46" s="3"/>
-    </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX46" s="3"/>
+      <c r="AY46" s="6"/>
+      <c r="AZ46" s="3"/>
+    </row>
+    <row r="47" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3398,7 +3448,7 @@
       <c r="AE47" s="2"/>
       <c r="AF47" s="2"/>
       <c r="AG47" s="2"/>
-      <c r="AH47" s="3"/>
+      <c r="AH47" s="2"/>
       <c r="AI47" s="3"/>
       <c r="AJ47" s="3"/>
       <c r="AK47" s="3"/>
@@ -3407,21 +3457,22 @@
       <c r="AN47" s="3"/>
       <c r="AO47" s="3"/>
       <c r="AP47" s="3"/>
-      <c r="AQ47" s="3">
-        <v>1</v>
-      </c>
-      <c r="AR47" s="3"/>
+      <c r="AQ47" s="3"/>
+      <c r="AR47" s="3">
+        <v>1</v>
+      </c>
       <c r="AS47" s="3"/>
       <c r="AT47" s="3"/>
       <c r="AU47" s="1"/>
       <c r="AV47" s="3"/>
       <c r="AW47" s="3"/>
-      <c r="AX47" s="6"/>
-      <c r="AY47" s="3"/>
-    </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX47" s="3"/>
+      <c r="AY47" s="6"/>
+      <c r="AZ47" s="3"/>
+    </row>
+    <row r="48" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3455,7 +3506,7 @@
       <c r="AE48" s="2"/>
       <c r="AF48" s="2"/>
       <c r="AG48" s="2"/>
-      <c r="AH48" s="3"/>
+      <c r="AH48" s="2"/>
       <c r="AI48" s="3"/>
       <c r="AJ48" s="3"/>
       <c r="AK48" s="3"/>
@@ -3464,21 +3515,22 @@
       <c r="AN48" s="3"/>
       <c r="AO48" s="3"/>
       <c r="AP48" s="3"/>
-      <c r="AQ48" s="3">
-        <v>1</v>
-      </c>
-      <c r="AR48" s="3"/>
+      <c r="AQ48" s="3"/>
+      <c r="AR48" s="3">
+        <v>1</v>
+      </c>
       <c r="AS48" s="3"/>
       <c r="AT48" s="3"/>
       <c r="AU48" s="3"/>
       <c r="AV48" s="1"/>
       <c r="AW48" s="3"/>
-      <c r="AX48" s="6"/>
-      <c r="AY48" s="3"/>
-    </row>
-    <row r="49" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX48" s="3"/>
+      <c r="AY48" s="6"/>
+      <c r="AZ48" s="3"/>
+    </row>
+    <row r="49" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3512,7 +3564,7 @@
       <c r="AE49" s="2"/>
       <c r="AF49" s="2"/>
       <c r="AG49" s="2"/>
-      <c r="AH49" s="3"/>
+      <c r="AH49" s="2"/>
       <c r="AI49" s="3"/>
       <c r="AJ49" s="3"/>
       <c r="AK49" s="3"/>
@@ -3522,122 +3574,183 @@
       <c r="AO49" s="3"/>
       <c r="AP49" s="3"/>
       <c r="AQ49" s="3"/>
-      <c r="AR49" s="3"/>
+      <c r="AR49" s="3">
+        <v>1</v>
+      </c>
       <c r="AS49" s="3"/>
       <c r="AT49" s="3"/>
       <c r="AU49" s="3"/>
       <c r="AV49" s="3"/>
       <c r="AW49" s="1"/>
-      <c r="AX49" s="6"/>
-      <c r="AY49" s="3"/>
-    </row>
-    <row r="50" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="AX49" s="3"/>
+      <c r="AY49" s="6"/>
+      <c r="AZ49" s="3"/>
+    </row>
+    <row r="50" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2"/>
+      <c r="Y50" s="2"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="2"/>
+      <c r="AF50" s="2"/>
+      <c r="AG50" s="2"/>
+      <c r="AH50" s="2"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="3"/>
+      <c r="AK50" s="3"/>
+      <c r="AL50" s="3"/>
+      <c r="AM50" s="3"/>
+      <c r="AN50" s="3"/>
+      <c r="AO50" s="3"/>
+      <c r="AP50" s="3"/>
+      <c r="AQ50" s="3"/>
+      <c r="AR50" s="3"/>
+      <c r="AS50" s="3"/>
+      <c r="AT50" s="3"/>
+      <c r="AU50" s="3"/>
+      <c r="AV50" s="3"/>
+      <c r="AW50" s="3"/>
+      <c r="AX50" s="1"/>
+      <c r="AY50" s="6"/>
+      <c r="AZ50" s="3"/>
+    </row>
+    <row r="51" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="10"/>
-      <c r="T50" s="10"/>
-      <c r="U50" s="10"/>
-      <c r="V50" s="10"/>
-      <c r="W50" s="10"/>
-      <c r="X50" s="10"/>
-      <c r="Y50" s="10"/>
-      <c r="Z50" s="10"/>
-      <c r="AA50" s="10"/>
-      <c r="AB50" s="10"/>
-      <c r="AC50" s="10"/>
-      <c r="AD50" s="10"/>
-      <c r="AE50" s="10"/>
-      <c r="AF50" s="10"/>
-      <c r="AG50" s="10"/>
-      <c r="AH50" s="11"/>
-      <c r="AI50" s="11"/>
-      <c r="AJ50" s="11"/>
-      <c r="AK50" s="11"/>
-      <c r="AL50" s="11"/>
-      <c r="AM50" s="11"/>
-      <c r="AN50" s="11"/>
-      <c r="AO50" s="11"/>
-      <c r="AP50" s="11"/>
-      <c r="AQ50" s="11"/>
-      <c r="AR50" s="11"/>
-      <c r="AS50" s="11"/>
-      <c r="AT50" s="11"/>
-      <c r="AU50" s="11"/>
-      <c r="AV50" s="11"/>
-      <c r="AW50" s="11">
-        <v>1</v>
-      </c>
-      <c r="AX50" s="14"/>
-      <c r="AY50" s="3"/>
-    </row>
-    <row r="51" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="2"/>
-      <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
-      <c r="W51" s="2"/>
-      <c r="X51" s="2"/>
-      <c r="Y51" s="2"/>
-      <c r="Z51" s="2"/>
-      <c r="AA51" s="2"/>
-      <c r="AB51" s="2"/>
-      <c r="AC51" s="2"/>
-      <c r="AD51" s="2"/>
-      <c r="AE51" s="2"/>
-      <c r="AF51" s="2"/>
-      <c r="AG51" s="2"/>
-      <c r="AH51" s="2"/>
-      <c r="AI51" s="2"/>
-      <c r="AJ51" s="2"/>
-      <c r="AK51" s="2"/>
-      <c r="AL51" s="2"/>
-      <c r="AM51" s="2"/>
-      <c r="AN51" s="2"/>
-      <c r="AO51" s="2"/>
-      <c r="AP51" s="2"/>
-      <c r="AQ51" s="2"/>
-      <c r="AR51" s="2"/>
-      <c r="AS51" s="2"/>
-      <c r="AT51" s="2"/>
-      <c r="AU51" s="2"/>
-      <c r="AV51" s="2"/>
-      <c r="AW51" s="2"/>
-      <c r="AX51" s="2"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+      <c r="S51" s="10"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="10"/>
+      <c r="V51" s="10"/>
+      <c r="W51" s="10"/>
+      <c r="X51" s="10"/>
+      <c r="Y51" s="10"/>
+      <c r="Z51" s="10"/>
+      <c r="AA51" s="10"/>
+      <c r="AB51" s="10"/>
+      <c r="AC51" s="10"/>
+      <c r="AD51" s="10"/>
+      <c r="AE51" s="10"/>
+      <c r="AF51" s="10"/>
+      <c r="AG51" s="10"/>
+      <c r="AH51" s="10"/>
+      <c r="AI51" s="11"/>
+      <c r="AJ51" s="11"/>
+      <c r="AK51" s="11"/>
+      <c r="AL51" s="11"/>
+      <c r="AM51" s="11"/>
+      <c r="AN51" s="11"/>
+      <c r="AO51" s="11"/>
+      <c r="AP51" s="11"/>
+      <c r="AQ51" s="11"/>
+      <c r="AR51" s="11"/>
+      <c r="AS51" s="11"/>
+      <c r="AT51" s="11"/>
+      <c r="AU51" s="11"/>
+      <c r="AV51" s="11"/>
+      <c r="AW51" s="11"/>
+      <c r="AX51" s="11">
+        <v>1</v>
+      </c>
+      <c r="AY51" s="14"/>
+      <c r="AZ51" s="3"/>
+    </row>
+    <row r="52" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
+      <c r="X52" s="2"/>
+      <c r="Y52" s="2"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
+      <c r="AB52" s="2"/>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="2"/>
+      <c r="AE52" s="2"/>
+      <c r="AF52" s="2"/>
+      <c r="AG52" s="2"/>
+      <c r="AH52" s="2"/>
+      <c r="AI52" s="2"/>
+      <c r="AJ52" s="2"/>
+      <c r="AK52" s="2"/>
+      <c r="AL52" s="2"/>
+      <c r="AM52" s="2"/>
+      <c r="AN52" s="2"/>
+      <c r="AO52" s="2"/>
+      <c r="AP52" s="2"/>
+      <c r="AQ52" s="2"/>
+      <c r="AR52" s="2"/>
+      <c r="AS52" s="2"/>
+      <c r="AT52" s="2"/>
+      <c r="AU52" s="2"/>
+      <c r="AV52" s="2"/>
+      <c r="AW52" s="2"/>
+      <c r="AX52" s="2"/>
+      <c r="AY52" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>